<commit_message>
changes to column formats
</commit_message>
<xml_diff>
--- a/09_2024_02/3_output/leche_09_2024_02_final.xlsx
+++ b/09_2024_02/3_output/leche_09_2024_02_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuel/gdrive/prgrmmng/fundo_vt/fundovt_form2tab/09_2024_02/3_output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6C2356-58C6-F34C-97FA-ED5F29050460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE0FD4D-7196-F040-A396-231C51BB3139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet_1" sheetId="1" r:id="rId1"/>
@@ -837,6 +837,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$]d/mm/yy;@" x16r2:formatCode16="[$-en-CO,1]d/mm/yy;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -889,11 +892,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1235,7 +1239,7 @@
   <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1315,7 +1319,7 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C2" t="s">
@@ -1368,7 +1372,7 @@
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C3" t="s">
@@ -1421,7 +1425,7 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C4" t="s">
@@ -1474,7 +1478,7 @@
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C5" t="s">
@@ -1527,7 +1531,7 @@
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C6" t="s">
@@ -1580,7 +1584,7 @@
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C7" t="s">
@@ -1633,7 +1637,7 @@
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C8" t="s">
@@ -1686,7 +1690,7 @@
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C9" t="s">
@@ -1739,7 +1743,7 @@
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C10" t="s">
@@ -1792,7 +1796,7 @@
       <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C11" t="s">
@@ -1845,7 +1849,7 @@
       <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C12" t="s">
@@ -1898,7 +1902,7 @@
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C13" t="s">
@@ -1951,7 +1955,7 @@
       <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C14" t="s">
@@ -1986,7 +1990,7 @@
       <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C15" t="s">
@@ -2039,7 +2043,7 @@
       <c r="A16" t="s">
         <v>25</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C16" t="s">
@@ -2092,7 +2096,7 @@
       <c r="A17" t="s">
         <v>26</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C17" t="s">
@@ -2145,7 +2149,7 @@
       <c r="A18" t="s">
         <v>27</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C18" t="s">
@@ -2198,7 +2202,7 @@
       <c r="A19" t="s">
         <v>28</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C19" t="s">
@@ -2251,7 +2255,7 @@
       <c r="A20" t="s">
         <v>29</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C20" t="s">
@@ -2304,7 +2308,7 @@
       <c r="A21" t="s">
         <v>30</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C21" t="s">
@@ -2357,7 +2361,7 @@
       <c r="A22" t="s">
         <v>31</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C22" t="s">
@@ -2410,7 +2414,7 @@
       <c r="A23" t="s">
         <v>32</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C23" t="s">
@@ -2463,7 +2467,7 @@
       <c r="A24" t="s">
         <v>33</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C24" t="s">
@@ -2516,7 +2520,7 @@
       <c r="A25" t="s">
         <v>34</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C25" t="s">
@@ -2569,7 +2573,7 @@
       <c r="A26" t="s">
         <v>35</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C26" t="s">
@@ -2622,7 +2626,7 @@
       <c r="A27" t="s">
         <v>36</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C27" t="s">
@@ -2675,7 +2679,7 @@
       <c r="A28" t="s">
         <v>37</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C28" t="s">
@@ -2728,7 +2732,7 @@
       <c r="A29" t="s">
         <v>38</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C29" t="s">
@@ -2781,7 +2785,7 @@
       <c r="A30" t="s">
         <v>39</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C30" t="s">
@@ -2834,7 +2838,7 @@
       <c r="A31" t="s">
         <v>40</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C31" t="s">
@@ -2887,7 +2891,7 @@
       <c r="A32" t="s">
         <v>41</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C32" t="s">
@@ -2940,7 +2944,7 @@
       <c r="A33" t="s">
         <v>42</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C33" t="s">
@@ -2993,7 +2997,7 @@
       <c r="A34" t="s">
         <v>43</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>76</v>
       </c>
       <c r="C34" t="s">
@@ -3046,7 +3050,7 @@
       <c r="A35" t="s">
         <v>44</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C35" t="s">
@@ -3099,7 +3103,7 @@
       <c r="A36" t="s">
         <v>45</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C36" t="s">
@@ -3152,7 +3156,7 @@
       <c r="A37" t="s">
         <v>46</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C37" t="s">
@@ -3205,7 +3209,7 @@
       <c r="A38" t="s">
         <v>47</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C38" t="s">
@@ -3258,7 +3262,7 @@
       <c r="A39" t="s">
         <v>48</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>79</v>
       </c>
       <c r="C39" t="s">

</xml_diff>